<commit_message>
updated Parameter excel file
</commit_message>
<xml_diff>
--- a/Vergleich/Parameter.xlsx
+++ b/Vergleich/Parameter.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Daten/Studium/Master EE/Masterprojekt/Git-Repository/Limits-to-Growth-Masterprojekt-TH-Koeln-2022/Vergleich/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{187A95FB-CC8A-3741-94DA-FA1E50C82F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57B1A3F-BA96-9A4F-9479-88150DC26C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14520" xr2:uid="{3F5EE684-BD36-5A47-B2A5-759BDA655248}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -50,13 +50,34 @@
     <t>nri</t>
   </si>
   <si>
-    <t>FALSE</t>
-  </si>
-  <si>
     <t>dcfsn</t>
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>start_val</t>
+  </si>
+  <si>
+    <t>end_val</t>
+  </si>
+  <si>
+    <t>use_in_analysis</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>frpm</t>
+  </si>
+  <si>
+    <t>pl</t>
   </si>
 </sst>
 </file>
@@ -409,15 +430,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29C10D4-A7FE-8146-8F58-EF47C8273621}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,8 +451,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -436,17 +469,59 @@
         <v>1000000000000</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <f>B2</f>
+        <v>1000000000000</v>
+      </c>
+      <c r="E2" s="1">
+        <f>8*B2</f>
+        <v>8000000000000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.02</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>